<commit_message>
Organized docs folder and added updated gantt chartt print
</commit_message>
<xml_diff>
--- a/docs/SINF-Gantt-Chart.xlsx
+++ b/docs/SINF-Gantt-Chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EDD27C-AFE8-4F46-8329-103301E5CD5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F36F078-4236-4A11-A237-C332097849F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Task 3</t>
   </si>
@@ -81,18 +72,6 @@
   </si>
   <si>
     <t>TASK</t>
-  </si>
-  <si>
-    <t>SIMPLE GANTT CHART by Vertex42.com</t>
-  </si>
-  <si>
-    <t>https://www.vertex42.com/ExcelTemplates/simple-gantt-chart.html</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Project Lead</t>
   </si>
   <si>
     <t>Enter Company Name in cell B2.</t>
@@ -251,7 +230,7 @@
     <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="168" formatCode="d"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +354,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -633,7 +620,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -820,6 +807,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -839,9 +838,6 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -851,14 +847,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1102,6 +1092,117 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>70</xdr:col>
+      <xdr:colOff>135300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>100922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>71</xdr:col>
+      <xdr:colOff>100295</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>294311</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Gráfico 5" descr="Parar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3182D81-AC00-48F8-AFEC-325C53A86644}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2700000">
+          <a:off x="17911840" y="9435784"/>
+          <a:ext cx="193389" cy="192666"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>77392</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>108943</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>99537</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>302332</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Gráfico 6" descr="Parar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09E97BB4-F8A0-4CEA-8017-AD5234CB7DC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2700000">
+          <a:off x="10639717" y="4871842"/>
+          <a:ext cx="193389" cy="192592"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1370,269 +1471,261 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BZ31"/>
+  <dimension ref="A1:CB31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR2" sqref="AR2"/>
+      <selection pane="bottomLeft" activeCell="CB10" sqref="CB10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="2.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5546875" customWidth="1"/>
-    <col min="65" max="65" width="3.88671875" customWidth="1"/>
-    <col min="66" max="67" width="3.5546875" customWidth="1"/>
-    <col min="68" max="69" width="4.109375" customWidth="1"/>
-    <col min="70" max="71" width="3.44140625" customWidth="1"/>
-    <col min="72" max="72" width="3.33203125" customWidth="1"/>
-    <col min="73" max="73" width="3.44140625" customWidth="1"/>
-    <col min="74" max="74" width="3.33203125" customWidth="1"/>
-    <col min="75" max="75" width="3.6640625" customWidth="1"/>
-    <col min="76" max="76" width="3.33203125" customWidth="1"/>
-    <col min="77" max="78" width="3.44140625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.5703125" customWidth="1"/>
+    <col min="65" max="65" width="3.85546875" customWidth="1"/>
+    <col min="66" max="67" width="3.5703125" customWidth="1"/>
+    <col min="68" max="69" width="4.140625" customWidth="1"/>
+    <col min="70" max="71" width="3.42578125" customWidth="1"/>
+    <col min="72" max="72" width="3.28515625" customWidth="1"/>
+    <col min="73" max="73" width="3.42578125" customWidth="1"/>
+    <col min="74" max="74" width="3.28515625" customWidth="1"/>
+    <col min="75" max="75" width="3.7109375" customWidth="1"/>
+    <col min="76" max="76" width="3.28515625" customWidth="1"/>
+    <col min="77" max="78" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:80" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="4"/>
       <c r="F1" s="42"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:80" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
         <v>14</v>
       </c>
+      <c r="B2" s="65"/>
+      <c r="I2" s="46"/>
     </row>
-    <row r="2" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:80" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="72">
+      <c r="D3" s="74"/>
+      <c r="E3" s="76">
         <f>DATE(2020,10,23)</f>
         <v>44127</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="I3" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="75"/>
-      <c r="T3" s="75"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="75"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="75"/>
-      <c r="Z3" s="75"/>
-      <c r="AA3" s="75"/>
-      <c r="AB3" s="75"/>
-      <c r="AC3" s="75"/>
-      <c r="AD3" s="75"/>
-      <c r="AE3" s="75"/>
-      <c r="AF3" s="76"/>
-      <c r="AG3" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH3" s="78"/>
-      <c r="AI3" s="78"/>
-      <c r="AJ3" s="78"/>
-      <c r="AK3" s="78"/>
-      <c r="AL3" s="78"/>
-      <c r="AM3" s="78"/>
-      <c r="AN3" s="78"/>
-      <c r="AO3" s="78"/>
-      <c r="AP3" s="78"/>
-      <c r="AQ3" s="78"/>
-      <c r="AR3" s="78"/>
-      <c r="AS3" s="78"/>
-      <c r="AT3" s="78"/>
-      <c r="AU3" s="78"/>
-      <c r="AV3" s="78"/>
-      <c r="AW3" s="78"/>
-      <c r="AX3" s="78"/>
-      <c r="AY3" s="78"/>
-      <c r="AZ3" s="78"/>
-      <c r="BA3" s="78"/>
-      <c r="BB3" s="78"/>
-      <c r="BC3" s="78"/>
-      <c r="BD3" s="78"/>
-      <c r="BE3" s="78"/>
-      <c r="BF3" s="78"/>
-      <c r="BG3" s="78"/>
-      <c r="BH3" s="78"/>
-      <c r="BI3" s="78"/>
-      <c r="BJ3" s="78"/>
-      <c r="BK3" s="78"/>
-      <c r="BL3" s="78"/>
-      <c r="BM3" s="78"/>
-      <c r="BN3" s="78"/>
-      <c r="BO3" s="78"/>
-      <c r="BP3" s="78"/>
-      <c r="BQ3" s="78"/>
-      <c r="BR3" s="78"/>
-      <c r="BS3" s="79"/>
+      <c r="F3" s="76"/>
+      <c r="I3" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="78"/>
+      <c r="AB3" s="78"/>
+      <c r="AC3" s="78"/>
+      <c r="AD3" s="78"/>
+      <c r="AE3" s="78"/>
+      <c r="AF3" s="79"/>
+      <c r="AG3" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
+      <c r="AJ3" s="68"/>
+      <c r="AK3" s="68"/>
+      <c r="AL3" s="68"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+      <c r="AV3" s="68"/>
+      <c r="AW3" s="68"/>
+      <c r="AX3" s="68"/>
+      <c r="AY3" s="68"/>
+      <c r="AZ3" s="68"/>
+      <c r="BA3" s="68"/>
+      <c r="BB3" s="68"/>
+      <c r="BC3" s="68"/>
+      <c r="BD3" s="68"/>
+      <c r="BE3" s="68"/>
+      <c r="BF3" s="68"/>
+      <c r="BG3" s="68"/>
+      <c r="BH3" s="68"/>
+      <c r="BI3" s="68"/>
+      <c r="BJ3" s="68"/>
+      <c r="BK3" s="68"/>
+      <c r="BL3" s="68"/>
+      <c r="BM3" s="68"/>
+      <c r="BN3" s="68"/>
+      <c r="BO3" s="68"/>
+      <c r="BP3" s="68"/>
+      <c r="BQ3" s="68"/>
+      <c r="BR3" s="68"/>
+      <c r="BS3" s="69"/>
     </row>
-    <row r="4" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:80" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="70"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="66">
+      <c r="I4" s="70">
         <f>I5</f>
         <v>44123</v>
       </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="66">
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="70">
         <f>P5</f>
         <v>44130</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="68"/>
-      <c r="W4" s="66">
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="72"/>
+      <c r="W4" s="70">
         <f>W5</f>
         <v>44137</v>
       </c>
-      <c r="X4" s="67"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67"/>
-      <c r="AC4" s="68"/>
-      <c r="AD4" s="66">
+      <c r="X4" s="71"/>
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="71"/>
+      <c r="AB4" s="71"/>
+      <c r="AC4" s="72"/>
+      <c r="AD4" s="70">
         <f>AD5</f>
         <v>44144</v>
       </c>
-      <c r="AE4" s="67"/>
-      <c r="AF4" s="67"/>
-      <c r="AG4" s="67"/>
-      <c r="AH4" s="67"/>
-      <c r="AI4" s="67"/>
-      <c r="AJ4" s="68"/>
-      <c r="AK4" s="66">
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="72"/>
+      <c r="AK4" s="70">
         <f>AK5</f>
         <v>44151</v>
       </c>
-      <c r="AL4" s="67"/>
-      <c r="AM4" s="67"/>
-      <c r="AN4" s="67"/>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="67"/>
-      <c r="AQ4" s="68"/>
-      <c r="AR4" s="66">
+      <c r="AL4" s="71"/>
+      <c r="AM4" s="71"/>
+      <c r="AN4" s="71"/>
+      <c r="AO4" s="71"/>
+      <c r="AP4" s="71"/>
+      <c r="AQ4" s="72"/>
+      <c r="AR4" s="70">
         <f>AR5</f>
         <v>44158</v>
       </c>
-      <c r="AS4" s="67"/>
-      <c r="AT4" s="67"/>
-      <c r="AU4" s="67"/>
-      <c r="AV4" s="67"/>
-      <c r="AW4" s="67"/>
-      <c r="AX4" s="68"/>
-      <c r="AY4" s="66">
+      <c r="AS4" s="71"/>
+      <c r="AT4" s="71"/>
+      <c r="AU4" s="71"/>
+      <c r="AV4" s="71"/>
+      <c r="AW4" s="71"/>
+      <c r="AX4" s="72"/>
+      <c r="AY4" s="70">
         <f>AY5</f>
         <v>44165</v>
       </c>
-      <c r="AZ4" s="67"/>
-      <c r="BA4" s="67"/>
-      <c r="BB4" s="67"/>
-      <c r="BC4" s="67"/>
-      <c r="BD4" s="67"/>
-      <c r="BE4" s="68"/>
-      <c r="BF4" s="66">
+      <c r="AZ4" s="71"/>
+      <c r="BA4" s="71"/>
+      <c r="BB4" s="71"/>
+      <c r="BC4" s="71"/>
+      <c r="BD4" s="71"/>
+      <c r="BE4" s="72"/>
+      <c r="BF4" s="70">
         <f>BF5</f>
         <v>44172</v>
       </c>
-      <c r="BG4" s="67"/>
-      <c r="BH4" s="67"/>
-      <c r="BI4" s="67"/>
-      <c r="BJ4" s="67"/>
-      <c r="BK4" s="67"/>
-      <c r="BL4" s="68"/>
-      <c r="BM4" s="66">
+      <c r="BG4" s="71"/>
+      <c r="BH4" s="71"/>
+      <c r="BI4" s="71"/>
+      <c r="BJ4" s="71"/>
+      <c r="BK4" s="71"/>
+      <c r="BL4" s="72"/>
+      <c r="BM4" s="70">
         <f t="shared" ref="BM4" si="0">BM5</f>
         <v>44179</v>
       </c>
-      <c r="BN4" s="67"/>
-      <c r="BO4" s="67"/>
-      <c r="BP4" s="67"/>
-      <c r="BQ4" s="67"/>
-      <c r="BR4" s="67"/>
-      <c r="BS4" s="68"/>
-      <c r="BT4" s="66">
+      <c r="BN4" s="71"/>
+      <c r="BO4" s="71"/>
+      <c r="BP4" s="71"/>
+      <c r="BQ4" s="71"/>
+      <c r="BR4" s="71"/>
+      <c r="BS4" s="72"/>
+      <c r="BT4" s="70">
         <f t="shared" ref="BT4" si="1">BT5</f>
         <v>44186</v>
       </c>
-      <c r="BU4" s="67"/>
-      <c r="BV4" s="67"/>
-      <c r="BW4" s="67"/>
-      <c r="BX4" s="67"/>
-      <c r="BY4" s="67"/>
-      <c r="BZ4" s="68"/>
+      <c r="BU4" s="71"/>
+      <c r="BV4" s="71"/>
+      <c r="BW4" s="71"/>
+      <c r="BX4" s="71"/>
+      <c r="BY4" s="71"/>
+      <c r="BZ4" s="72"/>
     </row>
-    <row r="5" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
+        <v>22</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44123</v>
@@ -1914,9 +2007,9 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="6" spans="1:78" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:80" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>13</v>
@@ -2218,9 +2311,9 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:78" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:80" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" s="47"/>
       <c r="E7"/>
@@ -2299,12 +2392,12 @@
       <c r="BY7" s="39"/>
       <c r="BZ7" s="39"/>
     </row>
-    <row r="8" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C8" s="54"/>
       <c r="D8" s="19"/>
@@ -2386,15 +2479,15 @@
       <c r="BY8" s="39"/>
       <c r="BZ8" s="39"/>
     </row>
-    <row r="9" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" s="60" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D9" s="22">
         <v>1</v>
@@ -2483,15 +2576,15 @@
       <c r="BY9" s="39"/>
       <c r="BZ9" s="39"/>
     </row>
-    <row r="10" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" s="60" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="22">
         <v>1</v>
@@ -2579,14 +2672,15 @@
       <c r="BX10" s="39"/>
       <c r="BY10" s="39"/>
       <c r="BZ10" s="39"/>
+      <c r="CB10" s="80"/>
     </row>
-    <row r="11" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="44"/>
       <c r="B11" s="60" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" s="22">
         <v>1</v>
@@ -2672,13 +2766,13 @@
       <c r="BY11" s="39"/>
       <c r="BZ11" s="39"/>
     </row>
-    <row r="12" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="44"/>
       <c r="B12" s="60" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D12" s="22">
         <v>1</v>
@@ -2764,13 +2858,13 @@
       <c r="BY12" s="39"/>
       <c r="BZ12" s="39"/>
     </row>
-    <row r="13" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="44"/>
       <c r="B13" s="60" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D13" s="22">
         <v>1</v>
@@ -2856,13 +2950,13 @@
       <c r="BY13" s="39"/>
       <c r="BZ13" s="39"/>
     </row>
-    <row r="14" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="43"/>
       <c r="B14" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="66" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>46</v>
       </c>
       <c r="D14" s="22">
         <v>1</v>
@@ -2951,12 +3045,12 @@
       <c r="BY14" s="39"/>
       <c r="BZ14" s="39"/>
     </row>
-    <row r="15" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="55"/>
       <c r="D15" s="24"/>
@@ -3038,16 +3132,16 @@
       <c r="BY15" s="39"/>
       <c r="BZ15" s="39"/>
     </row>
-    <row r="16" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:80" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="44"/>
       <c r="B16" s="61" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D16" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="51">
         <f>F14+1</f>
@@ -3133,16 +3227,16 @@
       <c r="BY16" s="39"/>
       <c r="BZ16" s="39"/>
     </row>
-    <row r="17" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="43"/>
       <c r="B17" s="61" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D17" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="51">
         <f>F16</f>
@@ -3228,16 +3322,16 @@
       <c r="BY17" s="39"/>
       <c r="BZ17" s="39"/>
     </row>
-    <row r="18" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="43"/>
       <c r="B18" s="61" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="51">
         <f>E17+7</f>
@@ -3323,16 +3417,16 @@
       <c r="BY18" s="39"/>
       <c r="BZ18" s="39"/>
     </row>
-    <row r="19" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="43"/>
       <c r="B19" s="61" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="51">
         <f>E18+7</f>
@@ -3418,16 +3512,16 @@
       <c r="BY19" s="39"/>
       <c r="BZ19" s="39"/>
     </row>
-    <row r="20" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="43"/>
       <c r="B20" s="61" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="51">
         <f>E19</f>
@@ -3510,12 +3604,12 @@
       <c r="BY20" s="39"/>
       <c r="BZ20" s="39"/>
     </row>
-    <row r="21" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="43" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C21" s="57"/>
       <c r="D21" s="29"/>
@@ -3597,16 +3691,16 @@
       <c r="BY21" s="39"/>
       <c r="BZ21" s="39"/>
     </row>
-    <row r="22" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="43"/>
       <c r="B22" s="62" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D22" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="52">
         <f>F20-1</f>
@@ -3692,16 +3786,16 @@
       <c r="BY22" s="39"/>
       <c r="BZ22" s="39"/>
     </row>
-    <row r="23" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="43"/>
       <c r="B23" s="62" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D23" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="52">
         <f>E22+3</f>
@@ -3787,16 +3881,16 @@
       <c r="BY23" s="39"/>
       <c r="BZ23" s="39"/>
     </row>
-    <row r="24" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="B24" s="62" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D24" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="52">
         <f>E23+2</f>
@@ -3882,16 +3976,16 @@
       <c r="BY24" s="39"/>
       <c r="BZ24" s="39"/>
     </row>
-    <row r="25" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="43"/>
       <c r="B25" s="62" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D25" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="52">
         <f t="shared" ref="E25" si="20">E24</f>
@@ -3977,16 +4071,16 @@
       <c r="BY25" s="39"/>
       <c r="BZ25" s="39"/>
     </row>
-    <row r="26" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="43"/>
       <c r="B26" s="62" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D26" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="52">
         <f>E24+2</f>
@@ -4072,9 +4166,9 @@
       <c r="BY26" s="39"/>
       <c r="BZ26" s="39"/>
     </row>
-    <row r="27" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="43" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B27" s="63"/>
       <c r="C27" s="59"/>
@@ -4157,9 +4251,9 @@
       <c r="BY27" s="39"/>
       <c r="BZ27" s="39"/>
     </row>
-    <row r="28" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="44" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B28" s="33" t="s">
         <v>5</v>
@@ -4244,33 +4338,33 @@
       <c r="BY28" s="41"/>
       <c r="BZ28" s="41"/>
     </row>
-    <row r="29" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="14"/>
       <c r="F30" s="45"/>
     </row>
-    <row r="31" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AG3:BS3"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="I3:AF3"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
@@ -4306,16 +4400,13 @@
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>